<commit_message>
Update: review corrections and change requests implemented and deliverables generated
</commit_message>
<xml_diff>
--- a/Design-Files/ACF_Out-v2.0/Deliverables/_BOM/Client_BOM_ACF_Out-v2.0.xlsx
+++ b/Design-Files/ACF_Out-v2.0/Deliverables/_BOM/Client_BOM_ACF_Out-v2.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\aSim Data\GitHub\stephenlong-acfoutputpcb\Design-Files\ACF_Out-v1.0\Deliverables\_BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eSpark Cons Group\Documents\GitHub\Melih-SoundSensor\stephenlong-acfoutputpcb\Design-Files\ACF_Out-v2.0\Deliverables\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE89D00C-A3F4-4D5D-A94B-0658EC03151B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2C0937-F28E-42DE-B408-6AFDC162F84D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="93">
   <si>
     <t>#</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Capacitor</t>
   </si>
   <si>
-    <t>Capacitors</t>
-  </si>
-  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -49,12 +46,6 @@
     <t>Headers and Wire Housings</t>
   </si>
   <si>
-    <t>Terminal Block</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -64,18 +55,9 @@
     <t>RJ45 Transformer</t>
   </si>
   <si>
-    <t>IC</t>
-  </si>
-  <si>
     <t>Designator</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>C3, C8</t>
   </si>
   <si>
@@ -106,12 +88,6 @@
     <t>J7</t>
   </si>
   <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
     <t>LED1, LED2</t>
   </si>
   <si>
@@ -133,18 +109,9 @@
     <t>T1, T2</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>CAP CER 22UF 25V X5R 0805</t>
-  </si>
-  <si>
-    <t>CAP CER 2.2UF 50V X7R 0805</t>
-  </si>
-  <si>
     <t>CAP CER 0.022UF 50V X7R 0603</t>
   </si>
   <si>
@@ -172,12 +139,6 @@
     <t>CONN HEADER R/A 8POS 3MM</t>
   </si>
   <si>
-    <t>TERM BLK 2POS SIDE ENTRY 5MM PCB</t>
-  </si>
-  <si>
-    <t>FIXED IND 10UH 1A 540 MOHM SMD</t>
-  </si>
-  <si>
     <t>515nm~525nm -30℃~+85℃ Emerald 30° 200mW Plugin,D=3mm Light Emitting Diodes (LED) ROHS</t>
   </si>
   <si>
@@ -199,15 +160,9 @@
     <t>XFRMR MAGNETIC 1PORT 1:1 10/100</t>
   </si>
   <si>
-    <t>IC REG BUCK 3.3V 500MA 10WSON</t>
-  </si>
-  <si>
     <t>Footprint</t>
   </si>
   <si>
-    <t>Cap-0805</t>
-  </si>
-  <si>
     <t>Cap-0603</t>
   </si>
   <si>
@@ -229,9 +184,6 @@
     <t>NE8FBV-C5-LED</t>
   </si>
   <si>
-    <t>IND-1008 (2520 Metric)</t>
-  </si>
-  <si>
     <t>TH LED 3mm_</t>
   </si>
   <si>
@@ -244,18 +196,9 @@
     <t>H1102NLT</t>
   </si>
   <si>
-    <t>10-WSON (3x2)</t>
-  </si>
-  <si>
     <t>Manufacturer Part Number</t>
   </si>
   <si>
-    <t>CC0805MKX5R8BB226</t>
-  </si>
-  <si>
-    <t>CC0805KKX7R9BB225</t>
-  </si>
-  <si>
     <t>CC0603KRX7R9BB223</t>
   </si>
   <si>
@@ -274,9 +217,6 @@
     <t>43045-0800</t>
   </si>
   <si>
-    <t>VLS252012HBX-100M-1</t>
-  </si>
-  <si>
     <t>NFD3401UGD</t>
   </si>
   <si>
@@ -298,9 +238,6 @@
     <t>H1102NL</t>
   </si>
   <si>
-    <t>TPS62177DQCR</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -322,27 +259,15 @@
     <t>Molex</t>
   </si>
   <si>
-    <t>TDK</t>
-  </si>
-  <si>
     <t>Foshan NationStar Optoelectronics</t>
   </si>
   <si>
     <t>Pulse</t>
   </si>
   <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>22uF</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
     <t>22nF</t>
   </si>
   <si>
@@ -353,9 +278,6 @@
   </si>
   <si>
     <t>10nF</t>
-  </si>
-  <si>
-    <t>10uH</t>
   </si>
   <si>
     <t>Emerald</t>
@@ -869,10 +791,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="K2" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,25 +831,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -940,56 +862,56 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="J3" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="11">
-        <f t="shared" ref="B4:B24" si="0">ROW(B4) - ROW($B$2)</f>
+        <f t="shared" ref="B4:B18" si="0">ROW(B4) - ROW($B$2)</f>
         <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="J4" s="9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1002,22 +924,22 @@
         <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="J5" s="7">
         <v>2</v>
@@ -1033,25 +955,25 @@
         <v>2</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>79</v>
-      </c>
       <c r="H6" s="9" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="J6" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1061,25 +983,25 @@
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="J7" s="7">
         <v>2</v>
@@ -1092,93 +1014,93 @@
         <v>6</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="J8" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="11">
         <f>ROW(B9) - ROW($B$2)</f>
         <v>7</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="J9" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="J10" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="11">
         <f>ROW(B11) - ROW($B$2)</f>
@@ -1188,53 +1110,53 @@
         <v>6</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="J11" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>67</v>
+        <v>38</v>
+      </c>
+      <c r="F12" s="9">
+        <v>430450800</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J12" s="9">
         <v>1</v>
@@ -1247,31 +1169,31 @@
         <v>11</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="J13" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="11">
         <f t="shared" si="0"/>
@@ -1281,28 +1203,28 @@
         <v>8</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="9">
-        <v>430450800</v>
+        <v>40</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J14" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="11">
         <f>ROW(B15) - ROW($B$2)</f>
@@ -1312,21 +1234,25 @@
         <v>9</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="7">
-        <v>691137710002</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8">
-        <v>691137710002</v>
+        <v>41</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="J15" s="7">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1336,276 +1262,121 @@
         <v>14</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="J16" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="11">
         <f>ROW(B17) - ROW($B$2)</f>
         <v>15</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="J17" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>11</v>
+      <c r="C18" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="J18" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="11">
         <f>ROW(B19) - ROW($B$2)</f>
         <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="J19" s="7">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="11">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="J20" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="11">
-        <f>ROW(B21) - ROW($B$2)</f>
-        <v>19</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="J21" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="11">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J22" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="11">
-        <f>ROW(B23) - ROW($B$2)</f>
-        <v>21</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="J23" s="7">
         <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="11">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="J24" s="9">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>